<commit_message>
Added new worflows. working on sending email to each candidate
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ionut-mihai.nicula\Documents\UiPath\UiPath Projects Assigned\[Internal]USN Robot\USN_AddNewPartnerRecommendation.1.0.2\lib\net45\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ionut-mihai.nicula\Documents\UiPath\UiPath Projects Assigned\[Internal]USN Robot\USN_AddNewEmployeeCertifications\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC33613-B4D3-4E13-8535-07352D7F36F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB63D619-2881-4305-B1A5-115F37BF0801}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -141,6 +141,84 @@
   </si>
   <si>
     <t>USNAddNewCandidate_LastCreatedAt</t>
+  </si>
+  <si>
+    <t>JOTDevBioId</t>
+  </si>
+  <si>
+    <t>USNRobot_JOTDevBioId</t>
+  </si>
+  <si>
+    <t>JOTBaBioId</t>
+  </si>
+  <si>
+    <t>USNRobot_JOTBaBioId</t>
+  </si>
+  <si>
+    <t>JOTSaBioId</t>
+  </si>
+  <si>
+    <t>USNRobot_JOTSaBioId</t>
+  </si>
+  <si>
+    <t>JOTInfraBioId</t>
+  </si>
+  <si>
+    <t>USNRobot_JOTInfraBioId</t>
+  </si>
+  <si>
+    <t>ValidNumberOfDays</t>
+  </si>
+  <si>
+    <t>UsnRobot_ValidNumberOfDays</t>
+  </si>
+  <si>
+    <t>EmailSubject4</t>
+  </si>
+  <si>
+    <t>UsnRobot_EmailSubject4</t>
+  </si>
+  <si>
+    <t>EmailBody4</t>
+  </si>
+  <si>
+    <t>UsnRobot_EmailBody4</t>
+  </si>
+  <si>
+    <t>EvaluatorEmail4</t>
+  </si>
+  <si>
+    <t>UsnRobot_EvaluatorEmail4</t>
+  </si>
+  <si>
+    <t>ForceInvite</t>
+  </si>
+  <si>
+    <t>UsnRobot_ForceInvite</t>
+  </si>
+  <si>
+    <t>DevTestID</t>
+  </si>
+  <si>
+    <t>UsnRobot_DevTestID</t>
+  </si>
+  <si>
+    <t>SATestID</t>
+  </si>
+  <si>
+    <t>UsnRobot_SATestID</t>
+  </si>
+  <si>
+    <t>BATestID</t>
+  </si>
+  <si>
+    <t>UsnRobot_BATestID</t>
+  </si>
+  <si>
+    <t>InfraTestID</t>
+  </si>
+  <si>
+    <t>UsnRobot_InfraTestID</t>
   </si>
 </sst>
 </file>
@@ -2700,7 +2778,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2769,34 +2847,125 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updated config file and added playground file for tests
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ionut-mihai.nicula\Documents\UiPath\UiPath Projects Assigned\[Internal]USN Robot\USN_AddNewEmployeeCertifications\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E381C76-A109-496A-991D-67882599ADDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A5B3DE-01AE-4E76-9FAC-B603199078E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t>USNAddNewCandidate_CandidateBioEmailSubject</t>
+  </si>
+  <si>
+    <t>USNAddNewCandidate_CandidateBioEmail_FormUrlPlaceholder</t>
+  </si>
+  <si>
+    <t>CandidateBioFormUrlPlaceholder</t>
   </si>
 </sst>
 </file>
@@ -2828,7 +2834,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3065,7 +3071,14 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
added dev/prod conection. mode in Config File if is dev it will use the dev conncetion
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ionut-mihai.nicula\Documents\UiPath\UiPath Projects Assigned\[Internal]USN Robot\USN_AddNewEmployeeCertifications\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B512F1FF-705D-4C88-B870-E925B65DEEEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCA72C9-5B04-40A3-9485-255EF8279835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -303,13 +303,31 @@
   </si>
   <si>
     <t>&lt;br&gt;&lt;p&gt;&lt;strong&gt;#infraBio#&lt;/strong&gt;&lt;/p&gt;#infraRow#</t>
+  </si>
+  <si>
+    <t>dbProd</t>
+  </si>
+  <si>
+    <t>Data Source=proj-usn-sql-serv.database.windows.net;Initial Catalog=proj-usn-db;Persist Security Info=True;User ID=bogdan;Password=B3uqzDSy|V4.doY</t>
+  </si>
+  <si>
+    <t>dev</t>
+  </si>
+  <si>
+    <t>dbDev</t>
+  </si>
+  <si>
+    <t>Data Source=proj-usn-sql-serv.database.windows.net;Initial Catalog=dev-proj-usn;Persist Security Info=True;User ID=bogdan;Password=B3uqzDSy|V4.doY</t>
+  </si>
+  <si>
+    <t>mode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -334,6 +352,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -355,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -365,6 +389,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1753,7 +1778,7 @@
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1911,22 +1936,45 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2885,6 +2933,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added insert into robot log for bio reminder. added dev formID and using it in dev mode
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ionut-mihai.nicula\Documents\UiPath\UiPath Projects Assigned\[Internal]USN Robot\USN_AddNewEmployeeCertifications\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCA72C9-5B04-40A3-9485-255EF8279835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FCCA67-E2F4-4600-8FD9-185A90007CDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
   <si>
     <t>Name</t>
   </si>
@@ -131,9 +131,6 @@
     <t>apiKey</t>
   </si>
   <si>
-    <t>FormID</t>
-  </si>
-  <si>
     <t>USNAddNewPartner_apiKey</t>
   </si>
   <si>
@@ -321,6 +318,15 @@
   </si>
   <si>
     <t>mode</t>
+  </si>
+  <si>
+    <t>ProdFormID</t>
+  </si>
+  <si>
+    <t>DevFormId</t>
+  </si>
+  <si>
+    <t>202092041237342</t>
   </si>
 </sst>
 </file>
@@ -389,7 +395,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1778,7 +1784,7 @@
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1906,63 +1912,68 @@
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" t="s">
         <v>92</v>
-      </c>
-      <c r="B18" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
-      <c r="B21" s="5"/>
+      <c r="A21" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2942,7 +2953,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2992,15 +3003,15 @@
         <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -3008,191 +3019,191 @@
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
         <v>38</v>
-      </c>
-      <c r="B5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
         <v>40</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
         <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
         <v>46</v>
-      </c>
-      <c r="B9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
         <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
         <v>50</v>
-      </c>
-      <c r="B11" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
         <v>52</v>
-      </c>
-      <c r="B12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
         <v>54</v>
-      </c>
-      <c r="B13" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
         <v>56</v>
-      </c>
-      <c r="B14" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
         <v>58</v>
-      </c>
-      <c r="B15" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
         <v>60</v>
-      </c>
-      <c r="B16" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
         <v>62</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>